<commit_message>
Actualización de Procedimientos 28/03/2025
</commit_message>
<xml_diff>
--- a/senosiain/Horas/horas-quincena 2 Marzo 2025.xlsx
+++ b/senosiain/Horas/horas-quincena 2 Marzo 2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fortia\Senosian\Horas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fortia\senosiain\Horas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220786BC-F140-4938-95E5-DD0A6BD04B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767EFCA7-83E0-4632-8992-FDD08ED04E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>fecha</t>
   </si>
@@ -99,20 +99,76 @@
   </si>
   <si>
     <t>Generación de Script para actualización de variables de trabajador</t>
+  </si>
+  <si>
+    <t>Se ajusta el procedimiento sp_alta_saldos_vacaciones.</t>
+  </si>
+  <si>
+    <t>Se actualiza la variable_01 de los sistemas de antiguedad que tenga valor nulo.</t>
+  </si>
+  <si>
+    <t>Se actualizan el valor de las vacaciones vencidas a un lote de trabajador</t>
+  </si>
+  <si>
+    <t>Se analiza el bugs en la programación de vacaciones donde los registros se inserta como vacaciones normales asi este</t>
+  </si>
+  <si>
+    <t>seleccionado vacaciones anticipadas, procedimiento sp_alta_programacion_vac</t>
+  </si>
+  <si>
+    <t>Se ejecuta el script para la actualización de la variable del trabajador 5 (INFONAVIT)</t>
+  </si>
+  <si>
+    <t>Se compila el procedimiento sp_alta_programacion_vac, con ajustes.</t>
+  </si>
+  <si>
+    <t>Lilia hace pruebas de programación de vacaciones
+Anticipadas
+Normales
+Pruebas Ok</t>
+  </si>
+  <si>
+    <t>Juan Gabriel hace pruebas de programación de vacaciones. 
+Anticipadas
+Normales
+Pruebas Ok</t>
+  </si>
+  <si>
+    <t>Juan Gabriel hace pruebas de cambio de estatus en programación de vacaciones.  Pruebas Ok</t>
+  </si>
+  <si>
+    <t>Lilia requiere ajuste de la programacion de vacaciones a los Trabajadores 78469, 79169, 79359, 18454</t>
+  </si>
+  <si>
+    <t>Abono</t>
+  </si>
+  <si>
+    <t>Saldo</t>
+  </si>
+  <si>
+    <t>Ajuste del procedimiento sp_alta_programacion_vac, para el manejo de las vacaciones colectivas.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -160,6 +216,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -197,49 +259,57 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -290,7 +360,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A2:E26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A2:E33">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="fecha" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora Inicio"/>
@@ -500,17 +570,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H986"/>
+  <dimension ref="A1:H994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" style="13" customWidth="1"/>
     <col min="2" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" customWidth="1"/>
     <col min="5" max="5" width="99" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7265625" customWidth="1"/>
     <col min="7" max="7" width="33.7265625" customWidth="1"/>
@@ -518,13 +588,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
@@ -687,102 +757,214 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
+      <c r="A17" s="12">
+        <v>45742</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D17" s="3">
+        <v>4</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="14"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="17" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="12"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="12">
+        <v>45743</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D23" s="3">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="12"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E24" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="12"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="18" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="11"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="12"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="12"/>
+      <c r="B28" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D28" s="3">
+        <v>4</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="12"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="12"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="12"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="12"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="11"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="10">
-        <f>SUBTOTAL(109,D3:D25)</f>
-        <v>9</v>
-      </c>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="D33" s="10">
+        <f>SUBTOTAL(109,D3:D32)</f>
+        <v>19</v>
+      </c>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D35" s="19">
+        <f>+D33*500</f>
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="13">
+        <v>45743</v>
+      </c>
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="20">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D38" s="20"/>
+    </row>
+    <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" s="20">
+        <f>+D35-D37</f>
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -941,14 +1123,14 @@
     <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1721,6 +1903,14 @@
     <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>